<commit_message>
Modified some formatting in nexcel
</commit_message>
<xml_diff>
--- a/billing_software/Sample_Template.xlsx
+++ b/billing_software/Sample_Template.xlsx
@@ -195,8 +195,8 @@
   </sheetPr>
   <dimension ref="A1:AU9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AU3" activeCellId="0" sqref="AU3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -364,101 +364,101 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1</v>
+        <v>1.999</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="T2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="U2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="V2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="W2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="X2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="Y2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="Z2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AA2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AB2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AC2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AE2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AF2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AG2" s="1" t="n">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="AH2" s="1" t="n">
         <f aca="false">SUM(C2:AG2)</f>
-        <v>31</v>
+        <v>61.699</v>
       </c>
       <c r="AI2" s="1" t="n">
         <v>0</v>
@@ -471,17 +471,17 @@
       </c>
       <c r="AL2" s="1" t="n">
         <f aca="false">IF(AK2="G", PRODUCT(AH2, $AP$2), PRODUCT(AH2, $AQ$2))</f>
-        <v>1426</v>
+        <v>2591.358</v>
       </c>
       <c r="AM2" s="1" t="n">
         <v>10</v>
       </c>
       <c r="AN2" s="1" t="n">
         <f aca="false">SUM(AL2, AL3, AI2, AJ2, AM2)</f>
-        <v>1696</v>
+        <v>2861.358</v>
       </c>
       <c r="AP2" s="1" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AQ2" s="1" t="n">
         <v>52</v>
@@ -493,10 +493,10 @@
         <v>480</v>
       </c>
       <c r="AT2" s="3" t="n">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="AU2" s="3" t="n">
-        <v>43344</v>
+        <v>43390</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,14 +633,14 @@
       </c>
       <c r="AL4" s="1" t="n">
         <f aca="false">IF(AK4="G", PRODUCT(AH4, $AP$2), PRODUCT(AH4, $AQ$2))</f>
-        <v>3413.2</v>
+        <v>3116.4</v>
       </c>
       <c r="AM4" s="1" t="n">
         <v>100</v>
       </c>
       <c r="AN4" s="1" t="n">
         <f aca="false">SUM(AL4, AL5, AI4, AJ4, AM4)</f>
-        <v>3917.2</v>
+        <v>3620.4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,7 +781,7 @@
       </c>
       <c r="AN6" s="1" t="n">
         <f aca="false">SUM(AL6, AL7, AI6, AJ6, AM6)</f>
-        <v>5370</v>
+        <v>5354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,7 +803,7 @@
       </c>
       <c r="AL7" s="1" t="n">
         <f aca="false">IF(AK7="G", PRODUCT(AH7, $AP$2), PRODUCT(AH7, $AQ$2))</f>
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,14 +915,14 @@
       </c>
       <c r="AL8" s="1" t="n">
         <f aca="false">IF(AK8="G", PRODUCT(AH8, $AP$2), PRODUCT(AH8, $AQ$2))</f>
-        <v>2852</v>
+        <v>2604</v>
       </c>
       <c r="AM8" s="1" t="n">
         <v>100</v>
       </c>
       <c r="AN8" s="1" t="n">
         <f aca="false">SUM(AL8, AL9, AI8, AJ8, AM8)</f>
-        <v>4512</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>